<commit_message>
[Doc]_Update tiến độ code, doc, update UC
</commit_message>
<xml_diff>
--- a/WIP/Users/HuyenPT/Tiến độ viết doc.xlsx
+++ b/WIP/Users/HuyenPT/Tiến độ viết doc.xlsx
@@ -401,6 +401,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -422,10 +426,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -731,7 +731,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -740,6 +740,7 @@
     <col min="5" max="5" width="57.7109375" customWidth="1"/>
     <col min="6" max="6" width="13.5703125" style="14" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
@@ -761,7 +762,7 @@
       <c r="B5" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="18" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="8" t="s">
@@ -778,7 +779,7 @@
       <c r="B6" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="17"/>
+      <c r="D6" s="19"/>
       <c r="E6" s="9" t="s">
         <v>59</v>
       </c>
@@ -793,7 +794,7 @@
       <c r="B7" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="17"/>
+      <c r="D7" s="19"/>
       <c r="E7" s="9" t="s">
         <v>58</v>
       </c>
@@ -808,7 +809,7 @@
       <c r="B8" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="D8" s="17"/>
+      <c r="D8" s="19"/>
       <c r="E8" s="9" t="s">
         <v>41</v>
       </c>
@@ -820,7 +821,7 @@
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D9" s="17"/>
+      <c r="D9" s="19"/>
       <c r="E9" s="9" t="s">
         <v>5</v>
       </c>
@@ -832,7 +833,7 @@
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D10" s="17"/>
+      <c r="D10" s="19"/>
       <c r="E10" s="9" t="s">
         <v>6</v>
       </c>
@@ -844,7 +845,7 @@
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D11" s="17"/>
+      <c r="D11" s="19"/>
       <c r="E11" s="9" t="s">
         <v>7</v>
       </c>
@@ -856,7 +857,7 @@
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D12" s="18"/>
+      <c r="D12" s="20"/>
       <c r="E12" s="9" t="s">
         <v>8</v>
       </c>
@@ -868,7 +869,7 @@
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="21" t="s">
         <v>14</v>
       </c>
       <c r="E13" s="3" t="s">
@@ -878,7 +879,7 @@
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D14" s="20"/>
+      <c r="D14" s="22"/>
       <c r="E14" s="3" t="s">
         <v>9</v>
       </c>
@@ -890,7 +891,7 @@
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D15" s="20"/>
+      <c r="D15" s="22"/>
       <c r="E15" s="3" t="s">
         <v>10</v>
       </c>
@@ -902,7 +903,7 @@
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D16" s="20"/>
+      <c r="D16" s="22"/>
       <c r="E16" s="4" t="s">
         <v>11</v>
       </c>
@@ -910,7 +911,7 @@
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D17" s="20"/>
+      <c r="D17" s="22"/>
       <c r="E17" s="4" t="s">
         <v>12</v>
       </c>
@@ -920,7 +921,7 @@
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D18" s="21"/>
+      <c r="D18" s="23"/>
       <c r="E18" s="4" t="s">
         <v>13</v>
       </c>
@@ -928,7 +929,7 @@
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D19" s="16" t="s">
+      <c r="D19" s="18" t="s">
         <v>19</v>
       </c>
       <c r="E19" s="9" t="s">
@@ -942,7 +943,7 @@
       </c>
     </row>
     <row r="20" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D20" s="17"/>
+      <c r="D20" s="19"/>
       <c r="E20" s="9" t="s">
         <v>16</v>
       </c>
@@ -954,7 +955,7 @@
       </c>
     </row>
     <row r="21" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D21" s="17"/>
+      <c r="D21" s="19"/>
       <c r="E21" s="9" t="s">
         <v>17</v>
       </c>
@@ -966,7 +967,7 @@
       </c>
     </row>
     <row r="22" spans="4:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D22" s="18"/>
+      <c r="D22" s="20"/>
       <c r="E22" s="9" t="s">
         <v>18</v>
       </c>
@@ -976,7 +977,7 @@
       <c r="G22" s="2"/>
     </row>
     <row r="23" spans="4:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="D23" s="19" t="s">
+      <c r="D23" s="21" t="s">
         <v>24</v>
       </c>
       <c r="E23" s="4" t="s">
@@ -990,7 +991,7 @@
       </c>
     </row>
     <row r="24" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D24" s="20"/>
+      <c r="D24" s="22"/>
       <c r="E24" s="4" t="s">
         <v>21</v>
       </c>
@@ -1000,7 +1001,7 @@
       <c r="G24" s="2"/>
     </row>
     <row r="25" spans="4:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="D25" s="20"/>
+      <c r="D25" s="22"/>
       <c r="E25" s="4" t="s">
         <v>22</v>
       </c>
@@ -1010,7 +1011,7 @@
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D26" s="21"/>
+      <c r="D26" s="23"/>
       <c r="E26" s="4" t="s">
         <v>23</v>
       </c>
@@ -1020,7 +1021,7 @@
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="18" t="s">
         <v>28</v>
       </c>
       <c r="E27" s="9" t="s">
@@ -1032,7 +1033,7 @@
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D28" s="17"/>
+      <c r="D28" s="19"/>
       <c r="E28" s="9" t="s">
         <v>26</v>
       </c>
@@ -1042,7 +1043,7 @@
       <c r="G28" s="2"/>
     </row>
     <row r="29" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D29" s="18"/>
+      <c r="D29" s="20"/>
       <c r="E29" s="9" t="s">
         <v>27</v>
       </c>
@@ -1052,7 +1053,7 @@
       <c r="G29" s="2"/>
     </row>
     <row r="30" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D30" s="22" t="s">
+      <c r="D30" s="24" t="s">
         <v>34</v>
       </c>
       <c r="E30" s="1" t="s">
@@ -1062,7 +1063,7 @@
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D31" s="22"/>
+      <c r="D31" s="24"/>
       <c r="E31" s="1" t="s">
         <v>30</v>
       </c>
@@ -1070,7 +1071,7 @@
       <c r="G31" s="2"/>
     </row>
     <row r="32" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D32" s="22"/>
+      <c r="D32" s="24"/>
       <c r="E32" s="1" t="s">
         <v>31</v>
       </c>
@@ -1078,7 +1079,7 @@
       <c r="G32" s="2"/>
     </row>
     <row r="33" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D33" s="22"/>
+      <c r="D33" s="24"/>
       <c r="E33" s="1" t="s">
         <v>32</v>
       </c>
@@ -1086,7 +1087,7 @@
       <c r="G33" s="2"/>
     </row>
     <row r="34" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D34" s="22"/>
+      <c r="D34" s="24"/>
       <c r="E34" s="2" t="s">
         <v>33</v>
       </c>
@@ -1094,10 +1095,10 @@
       <c r="G34" s="2"/>
     </row>
     <row r="35" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D35" s="16" t="s">
+      <c r="D35" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E35" s="24" t="s">
+      <c r="E35" s="17" t="s">
         <v>15</v>
       </c>
       <c r="F35" s="12" t="s">
@@ -1108,8 +1109,8 @@
       </c>
     </row>
     <row r="36" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D36" s="17"/>
-      <c r="E36" s="23" t="s">
+      <c r="D36" s="19"/>
+      <c r="E36" s="16" t="s">
         <v>37</v>
       </c>
       <c r="F36" s="12" t="s">
@@ -1123,7 +1124,7 @@
       </c>
     </row>
     <row r="37" spans="4:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="D37" s="17"/>
+      <c r="D37" s="19"/>
       <c r="E37" s="10" t="s">
         <v>39</v>
       </c>
@@ -1133,7 +1134,7 @@
       <c r="G37" s="2"/>
     </row>
     <row r="38" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D38" s="17"/>
+      <c r="D38" s="19"/>
       <c r="E38" s="10" t="s">
         <v>36</v>
       </c>
@@ -1143,7 +1144,7 @@
       <c r="G38" s="2"/>
     </row>
     <row r="39" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D39" s="17"/>
+      <c r="D39" s="19"/>
       <c r="E39" s="10" t="s">
         <v>38</v>
       </c>
@@ -1153,7 +1154,7 @@
       <c r="G39" s="2"/>
     </row>
     <row r="40" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D40" s="17"/>
+      <c r="D40" s="19"/>
       <c r="E40" s="6" t="s">
         <v>4</v>
       </c>
@@ -1165,7 +1166,7 @@
       </c>
     </row>
     <row r="41" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D41" s="17"/>
+      <c r="D41" s="19"/>
       <c r="E41" s="6" t="s">
         <v>40</v>
       </c>
@@ -1177,7 +1178,7 @@
       </c>
     </row>
     <row r="42" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D42" s="17"/>
+      <c r="D42" s="19"/>
       <c r="E42" s="6" t="s">
         <v>41</v>
       </c>
@@ -1189,7 +1190,7 @@
       </c>
     </row>
     <row r="43" spans="4:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="D43" s="17"/>
+      <c r="D43" s="19"/>
       <c r="E43" s="6" t="s">
         <v>42</v>
       </c>
@@ -1201,7 +1202,7 @@
       </c>
     </row>
     <row r="44" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D44" s="17"/>
+      <c r="D44" s="19"/>
       <c r="E44" s="6" t="s">
         <v>43</v>
       </c>
@@ -1209,8 +1210,8 @@
       <c r="G44" s="2"/>
     </row>
     <row r="45" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D45" s="17"/>
-      <c r="E45" s="23" t="s">
+      <c r="D45" s="19"/>
+      <c r="E45" s="16" t="s">
         <v>44</v>
       </c>
       <c r="F45" s="12" t="s">
@@ -1221,7 +1222,7 @@
       </c>
     </row>
     <row r="46" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D46" s="17"/>
+      <c r="D46" s="19"/>
       <c r="E46" s="10" t="s">
         <v>9</v>
       </c>
@@ -1233,7 +1234,7 @@
       </c>
     </row>
     <row r="47" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D47" s="17"/>
+      <c r="D47" s="19"/>
       <c r="E47" s="10" t="s">
         <v>45</v>
       </c>
@@ -1245,8 +1246,8 @@
       </c>
     </row>
     <row r="48" spans="4:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="D48" s="17"/>
-      <c r="E48" s="23" t="s">
+      <c r="D48" s="19"/>
+      <c r="E48" s="16" t="s">
         <v>46</v>
       </c>
       <c r="F48" s="13" t="s">
@@ -1260,15 +1261,15 @@
       </c>
     </row>
     <row r="49" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D49" s="17"/>
-      <c r="E49" s="23" t="s">
+      <c r="D49" s="19"/>
+      <c r="E49" s="16" t="s">
         <v>3</v>
       </c>
       <c r="F49" s="12"/>
       <c r="G49" s="2"/>
     </row>
     <row r="50" spans="4:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D50" s="18"/>
+      <c r="D50" s="20"/>
       <c r="E50" s="6" t="s">
         <v>47</v>
       </c>

</xml_diff>